<commit_message>
turn on the API
</commit_message>
<xml_diff>
--- a/Solution Files/sql_query.xlsx
+++ b/Solution Files/sql_query.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SQL Query" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="SQL Query" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG157"/>
+  <dimension ref="A1:AH157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,6 +591,11 @@
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
+          <t>period_value</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
           <t>aggregation</t>
         </is>
       </c>
@@ -711,6 +716,9 @@
         <v>0</v>
       </c>
       <c r="AG2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -830,6 +838,9 @@
         <v>0</v>
       </c>
       <c r="AG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -949,6 +960,9 @@
         <v>0</v>
       </c>
       <c r="AG4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1068,6 +1082,9 @@
         <v>0</v>
       </c>
       <c r="AG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1187,6 +1204,9 @@
         <v>0</v>
       </c>
       <c r="AG6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1306,6 +1326,9 @@
         <v>0</v>
       </c>
       <c r="AG7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1425,6 +1448,9 @@
         <v>0</v>
       </c>
       <c r="AG8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1544,6 +1570,9 @@
         <v>0</v>
       </c>
       <c r="AG9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1663,6 +1692,9 @@
         <v>0</v>
       </c>
       <c r="AG10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1782,6 +1814,9 @@
         <v>0</v>
       </c>
       <c r="AG11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1901,6 +1936,9 @@
         <v>0</v>
       </c>
       <c r="AG12" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2020,6 +2058,9 @@
         <v>0</v>
       </c>
       <c r="AG13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2139,6 +2180,9 @@
         <v>0</v>
       </c>
       <c r="AG14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2258,6 +2302,9 @@
         <v>0</v>
       </c>
       <c r="AG15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2377,6 +2424,9 @@
         <v>0</v>
       </c>
       <c r="AG16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2496,6 +2546,9 @@
         <v>0</v>
       </c>
       <c r="AG17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2615,6 +2668,9 @@
         <v>0</v>
       </c>
       <c r="AG18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2734,6 +2790,9 @@
         <v>0</v>
       </c>
       <c r="AG19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2853,6 +2912,9 @@
         <v>0</v>
       </c>
       <c r="AG20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2972,6 +3034,9 @@
         <v>0</v>
       </c>
       <c r="AG21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3091,6 +3156,9 @@
         <v>0</v>
       </c>
       <c r="AG22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3210,6 +3278,9 @@
         <v>0</v>
       </c>
       <c r="AG23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3329,6 +3400,9 @@
         <v>0</v>
       </c>
       <c r="AG24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3448,6 +3522,9 @@
         <v>0</v>
       </c>
       <c r="AG25" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3567,6 +3644,9 @@
         <v>0</v>
       </c>
       <c r="AG26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3686,6 +3766,9 @@
         <v>0</v>
       </c>
       <c r="AG27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3805,6 +3888,9 @@
         <v>0</v>
       </c>
       <c r="AG28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3924,6 +4010,9 @@
         <v>0</v>
       </c>
       <c r="AG29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4043,6 +4132,9 @@
         <v>0</v>
       </c>
       <c r="AG30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4162,6 +4254,9 @@
         <v>0</v>
       </c>
       <c r="AG31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4281,6 +4376,9 @@
         <v>0</v>
       </c>
       <c r="AG32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4400,6 +4498,9 @@
         <v>0</v>
       </c>
       <c r="AG33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4519,6 +4620,9 @@
         <v>0</v>
       </c>
       <c r="AG34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4638,6 +4742,9 @@
         <v>0</v>
       </c>
       <c r="AG35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4757,6 +4864,9 @@
         <v>0</v>
       </c>
       <c r="AG36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4876,6 +4986,9 @@
         <v>0</v>
       </c>
       <c r="AG37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4995,6 +5108,9 @@
         <v>0</v>
       </c>
       <c r="AG38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5114,6 +5230,9 @@
         <v>0</v>
       </c>
       <c r="AG39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5233,6 +5352,9 @@
         <v>0</v>
       </c>
       <c r="AG40" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5352,6 +5474,9 @@
         <v>0</v>
       </c>
       <c r="AG41" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5471,6 +5596,9 @@
         <v>0</v>
       </c>
       <c r="AG42" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5590,6 +5718,9 @@
         <v>0</v>
       </c>
       <c r="AG43" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5709,6 +5840,9 @@
         <v>0</v>
       </c>
       <c r="AG44" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5828,6 +5962,9 @@
         <v>0</v>
       </c>
       <c r="AG45" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5947,6 +6084,9 @@
         <v>0</v>
       </c>
       <c r="AG46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6066,6 +6206,9 @@
         <v>0</v>
       </c>
       <c r="AG47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6185,6 +6328,9 @@
         <v>0</v>
       </c>
       <c r="AG48" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6304,6 +6450,9 @@
         <v>0</v>
       </c>
       <c r="AG49" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6423,6 +6572,9 @@
         <v>0</v>
       </c>
       <c r="AG50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6542,6 +6694,9 @@
         <v>0</v>
       </c>
       <c r="AG51" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6661,6 +6816,9 @@
         <v>0</v>
       </c>
       <c r="AG52" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6780,6 +6938,9 @@
         <v>0</v>
       </c>
       <c r="AG53" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6899,6 +7060,9 @@
         <v>0</v>
       </c>
       <c r="AG54" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7018,6 +7182,9 @@
         <v>0</v>
       </c>
       <c r="AG55" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7137,6 +7304,9 @@
         <v>0</v>
       </c>
       <c r="AG56" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7256,6 +7426,9 @@
         <v>0</v>
       </c>
       <c r="AG57" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7375,6 +7548,9 @@
         <v>0</v>
       </c>
       <c r="AG58" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7494,6 +7670,9 @@
         <v>0</v>
       </c>
       <c r="AG59" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7613,6 +7792,9 @@
         <v>0</v>
       </c>
       <c r="AG60" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7732,6 +7914,9 @@
         <v>0</v>
       </c>
       <c r="AG61" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7851,6 +8036,9 @@
         <v>0</v>
       </c>
       <c r="AG62" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7970,6 +8158,9 @@
         <v>0</v>
       </c>
       <c r="AG63" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8089,6 +8280,9 @@
         <v>0</v>
       </c>
       <c r="AG64" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8208,6 +8402,9 @@
         <v>0</v>
       </c>
       <c r="AG65" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8327,6 +8524,9 @@
         <v>0</v>
       </c>
       <c r="AG66" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8446,6 +8646,9 @@
         <v>0</v>
       </c>
       <c r="AG67" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8565,6 +8768,9 @@
         <v>0</v>
       </c>
       <c r="AG68" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8684,6 +8890,9 @@
         <v>0</v>
       </c>
       <c r="AG69" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8803,6 +9012,9 @@
         <v>0</v>
       </c>
       <c r="AG70" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8922,6 +9134,9 @@
         <v>0</v>
       </c>
       <c r="AG71" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9041,6 +9256,9 @@
         <v>0</v>
       </c>
       <c r="AG72" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9160,6 +9378,9 @@
         <v>0</v>
       </c>
       <c r="AG73" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9279,6 +9500,9 @@
         <v>0</v>
       </c>
       <c r="AG74" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9398,6 +9622,9 @@
         <v>0</v>
       </c>
       <c r="AG75" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9517,6 +9744,9 @@
         <v>0</v>
       </c>
       <c r="AG76" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9636,6 +9866,9 @@
         <v>0</v>
       </c>
       <c r="AG77" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9755,6 +9988,9 @@
         <v>0</v>
       </c>
       <c r="AG78" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9874,6 +10110,9 @@
         <v>0</v>
       </c>
       <c r="AG79" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9993,6 +10232,9 @@
         <v>0</v>
       </c>
       <c r="AG80" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10112,6 +10354,9 @@
         <v>0</v>
       </c>
       <c r="AG81" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10231,6 +10476,9 @@
         <v>0</v>
       </c>
       <c r="AG82" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10350,6 +10598,9 @@
         <v>0</v>
       </c>
       <c r="AG83" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10469,6 +10720,9 @@
         <v>0</v>
       </c>
       <c r="AG84" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10588,6 +10842,9 @@
         <v>0</v>
       </c>
       <c r="AG85" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10707,6 +10964,9 @@
         <v>0</v>
       </c>
       <c r="AG86" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10826,6 +11086,9 @@
         <v>0</v>
       </c>
       <c r="AG87" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10945,6 +11208,9 @@
         <v>0</v>
       </c>
       <c r="AG88" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH88" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11064,6 +11330,9 @@
         <v>0</v>
       </c>
       <c r="AG89" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH89" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11183,6 +11452,9 @@
         <v>0</v>
       </c>
       <c r="AG90" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11302,6 +11574,9 @@
         <v>0</v>
       </c>
       <c r="AG91" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH91" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11421,6 +11696,9 @@
         <v>0</v>
       </c>
       <c r="AG92" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11540,6 +11818,9 @@
         <v>0</v>
       </c>
       <c r="AG93" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH93" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11659,6 +11940,9 @@
         <v>0</v>
       </c>
       <c r="AG94" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH94" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11778,6 +12062,9 @@
         <v>0</v>
       </c>
       <c r="AG95" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH95" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11897,6 +12184,9 @@
         <v>0</v>
       </c>
       <c r="AG96" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12016,6 +12306,9 @@
         <v>0</v>
       </c>
       <c r="AG97" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH97" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12135,6 +12428,9 @@
         <v>0</v>
       </c>
       <c r="AG98" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12254,6 +12550,9 @@
         <v>0</v>
       </c>
       <c r="AG99" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH99" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12373,6 +12672,9 @@
         <v>0</v>
       </c>
       <c r="AG100" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12492,6 +12794,9 @@
         <v>0</v>
       </c>
       <c r="AG101" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH101" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12611,6 +12916,9 @@
         <v>0</v>
       </c>
       <c r="AG102" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH102" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12730,6 +13038,9 @@
         <v>0</v>
       </c>
       <c r="AG103" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH103" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12849,6 +13160,9 @@
         <v>0</v>
       </c>
       <c r="AG104" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH104" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12968,6 +13282,9 @@
         <v>0</v>
       </c>
       <c r="AG105" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH105" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13087,6 +13404,9 @@
         <v>0</v>
       </c>
       <c r="AG106" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH106" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13206,6 +13526,9 @@
         <v>0</v>
       </c>
       <c r="AG107" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH107" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13325,6 +13648,9 @@
         <v>0</v>
       </c>
       <c r="AG108" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH108" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13444,6 +13770,9 @@
         <v>0</v>
       </c>
       <c r="AG109" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH109" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13563,6 +13892,9 @@
         <v>0</v>
       </c>
       <c r="AG110" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH110" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13682,6 +14014,9 @@
         <v>0</v>
       </c>
       <c r="AG111" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13801,6 +14136,9 @@
         <v>0</v>
       </c>
       <c r="AG112" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH112" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13920,6 +14258,9 @@
         <v>0</v>
       </c>
       <c r="AG113" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH113" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14039,6 +14380,9 @@
         <v>0</v>
       </c>
       <c r="AG114" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH114" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14158,6 +14502,9 @@
         <v>0</v>
       </c>
       <c r="AG115" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH115" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14277,6 +14624,9 @@
         <v>0</v>
       </c>
       <c r="AG116" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH116" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14396,6 +14746,9 @@
         <v>0</v>
       </c>
       <c r="AG117" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH117" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14515,6 +14868,9 @@
         <v>0</v>
       </c>
       <c r="AG118" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH118" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14634,6 +14990,9 @@
         <v>0</v>
       </c>
       <c r="AG119" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH119" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14753,6 +15112,9 @@
         <v>0</v>
       </c>
       <c r="AG120" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH120" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14872,6 +15234,9 @@
         <v>0</v>
       </c>
       <c r="AG121" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH121" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14991,6 +15356,9 @@
         <v>0</v>
       </c>
       <c r="AG122" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH122" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15110,6 +15478,9 @@
         <v>0</v>
       </c>
       <c r="AG123" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH123" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15229,6 +15600,9 @@
         <v>0</v>
       </c>
       <c r="AG124" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH124" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15348,6 +15722,9 @@
         <v>0</v>
       </c>
       <c r="AG125" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH125" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15467,6 +15844,9 @@
         <v>0</v>
       </c>
       <c r="AG126" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH126" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15586,6 +15966,9 @@
         <v>0</v>
       </c>
       <c r="AG127" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH127" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15705,6 +16088,9 @@
         <v>0</v>
       </c>
       <c r="AG128" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH128" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15824,6 +16210,9 @@
         <v>0</v>
       </c>
       <c r="AG129" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH129" t="n">
         <v>0</v>
       </c>
     </row>
@@ -15943,6 +16332,9 @@
         <v>0</v>
       </c>
       <c r="AG130" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH130" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16062,6 +16454,9 @@
         <v>0</v>
       </c>
       <c r="AG131" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH131" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16181,6 +16576,9 @@
         <v>0</v>
       </c>
       <c r="AG132" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH132" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16300,6 +16698,9 @@
         <v>0</v>
       </c>
       <c r="AG133" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH133" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16419,6 +16820,9 @@
         <v>0</v>
       </c>
       <c r="AG134" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH134" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16538,6 +16942,9 @@
         <v>0</v>
       </c>
       <c r="AG135" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH135" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16657,6 +17064,9 @@
         <v>0</v>
       </c>
       <c r="AG136" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH136" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16776,6 +17186,9 @@
         <v>0</v>
       </c>
       <c r="AG137" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH137" t="n">
         <v>0</v>
       </c>
     </row>
@@ -16895,6 +17308,9 @@
         <v>0</v>
       </c>
       <c r="AG138" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH138" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17014,6 +17430,9 @@
         <v>0</v>
       </c>
       <c r="AG139" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH139" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17133,6 +17552,9 @@
         <v>0</v>
       </c>
       <c r="AG140" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH140" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17252,6 +17674,9 @@
         <v>0</v>
       </c>
       <c r="AG141" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH141" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17371,6 +17796,9 @@
         <v>0</v>
       </c>
       <c r="AG142" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH142" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17490,6 +17918,9 @@
         <v>0</v>
       </c>
       <c r="AG143" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH143" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17609,6 +18040,9 @@
         <v>0</v>
       </c>
       <c r="AG144" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH144" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17728,6 +18162,9 @@
         <v>0</v>
       </c>
       <c r="AG145" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH145" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17847,6 +18284,9 @@
         <v>0</v>
       </c>
       <c r="AG146" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH146" t="n">
         <v>0</v>
       </c>
     </row>
@@ -17966,6 +18406,9 @@
         <v>0</v>
       </c>
       <c r="AG147" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH147" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18085,6 +18528,9 @@
         <v>0</v>
       </c>
       <c r="AG148" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH148" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18204,6 +18650,9 @@
         <v>0</v>
       </c>
       <c r="AG149" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH149" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18323,6 +18772,9 @@
         <v>0</v>
       </c>
       <c r="AG150" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH150" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18442,6 +18894,9 @@
         <v>0</v>
       </c>
       <c r="AG151" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH151" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18561,6 +19016,9 @@
         <v>0</v>
       </c>
       <c r="AG152" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH152" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18680,6 +19138,9 @@
         <v>0</v>
       </c>
       <c r="AG153" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH153" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18799,6 +19260,9 @@
         <v>0</v>
       </c>
       <c r="AG154" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH154" t="n">
         <v>0</v>
       </c>
     </row>
@@ -18918,6 +19382,9 @@
         <v>0</v>
       </c>
       <c r="AG155" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH155" t="n">
         <v>0</v>
       </c>
     </row>
@@ -19037,6 +19504,9 @@
         <v>0</v>
       </c>
       <c r="AG156" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH156" t="n">
         <v>0</v>
       </c>
     </row>
@@ -19156,6 +19626,9 @@
         <v>0</v>
       </c>
       <c r="AG157" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH157" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>